<commit_message>
Moved files from Eclipse project and ran a toy test run
</commit_message>
<xml_diff>
--- a/Baggie_case_deployments.xlsx
+++ b/Baggie_case_deployments.xlsx
@@ -5,12 +5,12 @@
   <workbookPr defaultThemeVersion="202300"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://stlawu-my.sharepoint.com/personal/adfaut22_stlawu_edu/Documents/SLU Senior/Bio SYE/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://stlawu-my.sharepoint.com/personal/adfaut22_stlawu_edu/Documents/SLU Senior/Bio SYE/BirdNet_Analysis/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{3E6427FB-A8B6-C946-8A75-8D4BAD813053}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="58" documentId="8_{3E6427FB-A8B6-C946-8A75-8D4BAD813053}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{5C46DDA3-3D5A-0445-B8B0-EC881FF8A2B7}"/>
   <bookViews>
-    <workbookView xWindow="680" yWindow="760" windowWidth="28040" windowHeight="17220" xr2:uid="{6921FA91-0B64-6A44-8982-A083623F1019}"/>
+    <workbookView xWindow="-32260" yWindow="3380" windowWidth="28040" windowHeight="17220" xr2:uid="{6921FA91-0B64-6A44-8982-A083623F1019}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="278" uniqueCount="159">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="306" uniqueCount="174">
   <si>
     <t>Aidan Fauth, Liz Anderson</t>
   </si>
@@ -513,6 +513,51 @@
   </si>
   <si>
     <t>FLAG_comments</t>
+  </si>
+  <si>
+    <t>A004_SD013</t>
+  </si>
+  <si>
+    <t>Not logged</t>
+  </si>
+  <si>
+    <t>A008_SD021</t>
+  </si>
+  <si>
+    <t>A009_SD012</t>
+  </si>
+  <si>
+    <t>A011_SD018</t>
+  </si>
+  <si>
+    <t>A014_SD005</t>
+  </si>
+  <si>
+    <t>A021_SD003</t>
+  </si>
+  <si>
+    <t>A024_SD004</t>
+  </si>
+  <si>
+    <t>A001_SD007</t>
+  </si>
+  <si>
+    <t>A002_SD030</t>
+  </si>
+  <si>
+    <t>A007_SD008</t>
+  </si>
+  <si>
+    <t>A010_SD019</t>
+  </si>
+  <si>
+    <t>A017_SD017</t>
+  </si>
+  <si>
+    <t>A025_SD006</t>
+  </si>
+  <si>
+    <t>A025_SD100</t>
   </si>
 </sst>
 </file>
@@ -588,12 +633,18 @@
       <family val="2"/>
     </font>
   </fonts>
-  <fills count="2">
+  <fills count="3">
     <fill>
       <patternFill patternType="none"/>
     </fill>
     <fill>
       <patternFill patternType="gray125"/>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFFF00"/>
+        <bgColor indexed="64"/>
+      </patternFill>
     </fill>
   </fills>
   <borders count="1">
@@ -608,7 +659,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="14">
+  <cellXfs count="15">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
@@ -623,6 +674,7 @@
     <xf numFmtId="0" fontId="9" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="11" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
     <xf numFmtId="0" fontId="10" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -638,6 +690,10 @@
     </ext>
   </extLst>
 </styleSheet>
+</file>
+
+<file path=xl/persons/person.xml><?xml version="1.0" encoding="utf-8"?>
+<personList xmlns="http://schemas.microsoft.com/office/spreadsheetml/2018/threadedcomments" xmlns:x="http://schemas.openxmlformats.org/spreadsheetml/2006/main"/>
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
@@ -957,10 +1013,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{444F1B8C-D88B-974C-9D0F-AA216AACE439}">
-  <dimension ref="A1:AI17"/>
+  <dimension ref="A1:AI31"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="O13" sqref="O13"/>
+      <selection activeCell="A17" sqref="A17"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -1079,7 +1135,7 @@
       <c r="B2" s="1" t="s">
         <v>5</v>
       </c>
-      <c r="C2" s="1">
+      <c r="C2" s="14">
         <v>24</v>
       </c>
       <c r="D2" s="1" t="s">
@@ -1170,7 +1226,7 @@
       <c r="B3" s="1" t="s">
         <v>5</v>
       </c>
-      <c r="C3" s="1">
+      <c r="C3" s="14">
         <v>3</v>
       </c>
       <c r="D3" s="1" t="s">
@@ -1265,7 +1321,7 @@
       <c r="B4" s="1" t="s">
         <v>5</v>
       </c>
-      <c r="C4" s="1">
+      <c r="C4" s="14">
         <v>16</v>
       </c>
       <c r="D4" s="1" t="s">
@@ -1358,7 +1414,7 @@
       <c r="B5" s="1" t="s">
         <v>5</v>
       </c>
-      <c r="C5" s="1">
+      <c r="C5" s="14">
         <v>23</v>
       </c>
       <c r="D5" s="1" t="s">
@@ -1451,7 +1507,7 @@
       <c r="B6" s="1" t="s">
         <v>5</v>
       </c>
-      <c r="C6" s="1">
+      <c r="C6" s="14">
         <v>18</v>
       </c>
       <c r="D6" s="12" t="s">
@@ -1542,7 +1598,7 @@
       <c r="B7" s="1" t="s">
         <v>5</v>
       </c>
-      <c r="C7" s="1">
+      <c r="C7" s="14">
         <v>7</v>
       </c>
       <c r="D7" s="1" t="s">
@@ -1635,7 +1691,7 @@
       <c r="AI7" s="1"/>
     </row>
     <row r="8" spans="1:35" x14ac:dyDescent="0.2">
-      <c r="A8" s="1" t="s">
+      <c r="A8" s="14" t="s">
         <v>44</v>
       </c>
       <c r="B8" s="1" t="s">
@@ -1734,7 +1790,7 @@
       </c>
     </row>
     <row r="9" spans="1:35" x14ac:dyDescent="0.2">
-      <c r="A9" s="1" t="s">
+      <c r="A9" s="14" t="s">
         <v>52</v>
       </c>
       <c r="B9" s="1" t="s">
@@ -1833,7 +1889,7 @@
       <c r="AI9" s="1"/>
     </row>
     <row r="10" spans="1:35" x14ac:dyDescent="0.2">
-      <c r="A10" s="1" t="s">
+      <c r="A10" s="14" t="s">
         <v>60</v>
       </c>
       <c r="B10" s="1" t="s">
@@ -1932,7 +1988,7 @@
       <c r="AI10" s="1"/>
     </row>
     <row r="11" spans="1:35" x14ac:dyDescent="0.2">
-      <c r="A11" s="1" t="s">
+      <c r="A11" s="14" t="s">
         <v>68</v>
       </c>
       <c r="B11" s="1" t="s">
@@ -2033,7 +2089,7 @@
       <c r="AI11" s="1"/>
     </row>
     <row r="12" spans="1:35" x14ac:dyDescent="0.2">
-      <c r="A12" s="1" t="s">
+      <c r="A12" s="14" t="s">
         <v>76</v>
       </c>
       <c r="B12" s="1" t="s">
@@ -2134,7 +2190,7 @@
       <c r="AI12" s="1"/>
     </row>
     <row r="13" spans="1:35" x14ac:dyDescent="0.2">
-      <c r="A13" s="1" t="s">
+      <c r="A13" s="14" t="s">
         <v>84</v>
       </c>
       <c r="B13" s="1" t="s">
@@ -2338,7 +2394,7 @@
       </c>
     </row>
     <row r="15" spans="1:35" x14ac:dyDescent="0.2">
-      <c r="A15" s="1" t="s">
+      <c r="A15" s="14" t="s">
         <v>100</v>
       </c>
       <c r="B15" s="1" t="s">
@@ -2439,7 +2495,7 @@
       </c>
     </row>
     <row r="16" spans="1:35" x14ac:dyDescent="0.2">
-      <c r="A16" s="1" t="s">
+      <c r="A16" s="14" t="s">
         <v>109</v>
       </c>
       <c r="B16" s="1" t="s">
@@ -2540,7 +2596,7 @@
       <c r="AI16" s="1"/>
     </row>
     <row r="17" spans="1:35" x14ac:dyDescent="0.2">
-      <c r="A17" s="1" t="s">
+      <c r="A17" s="14" t="s">
         <v>116</v>
       </c>
       <c r="B17" s="1" t="s">
@@ -2639,6 +2695,118 @@
         <v>0</v>
       </c>
       <c r="AI17" s="1"/>
+    </row>
+    <row r="18" spans="1:35" x14ac:dyDescent="0.2">
+      <c r="A18" s="14" t="s">
+        <v>159</v>
+      </c>
+      <c r="B18" s="1" t="s">
+        <v>160</v>
+      </c>
+    </row>
+    <row r="19" spans="1:35" x14ac:dyDescent="0.2">
+      <c r="A19" s="14" t="s">
+        <v>161</v>
+      </c>
+      <c r="B19" s="1" t="s">
+        <v>160</v>
+      </c>
+    </row>
+    <row r="20" spans="1:35" x14ac:dyDescent="0.2">
+      <c r="A20" s="14" t="s">
+        <v>162</v>
+      </c>
+      <c r="B20" s="1" t="s">
+        <v>160</v>
+      </c>
+    </row>
+    <row r="21" spans="1:35" x14ac:dyDescent="0.2">
+      <c r="A21" s="14" t="s">
+        <v>163</v>
+      </c>
+      <c r="B21" s="1" t="s">
+        <v>160</v>
+      </c>
+    </row>
+    <row r="22" spans="1:35" x14ac:dyDescent="0.2">
+      <c r="A22" s="14" t="s">
+        <v>164</v>
+      </c>
+      <c r="B22" s="1" t="s">
+        <v>160</v>
+      </c>
+    </row>
+    <row r="23" spans="1:35" x14ac:dyDescent="0.2">
+      <c r="A23" s="14" t="s">
+        <v>165</v>
+      </c>
+      <c r="B23" s="1" t="s">
+        <v>160</v>
+      </c>
+    </row>
+    <row r="24" spans="1:35" x14ac:dyDescent="0.2">
+      <c r="A24" s="14" t="s">
+        <v>166</v>
+      </c>
+      <c r="B24" s="1" t="s">
+        <v>160</v>
+      </c>
+    </row>
+    <row r="25" spans="1:35" x14ac:dyDescent="0.2">
+      <c r="A25" s="14" t="s">
+        <v>167</v>
+      </c>
+      <c r="B25" s="1" t="s">
+        <v>160</v>
+      </c>
+    </row>
+    <row r="26" spans="1:35" x14ac:dyDescent="0.2">
+      <c r="A26" s="14" t="s">
+        <v>168</v>
+      </c>
+      <c r="B26" s="1" t="s">
+        <v>160</v>
+      </c>
+    </row>
+    <row r="27" spans="1:35" x14ac:dyDescent="0.2">
+      <c r="A27" s="14" t="s">
+        <v>169</v>
+      </c>
+      <c r="B27" s="1" t="s">
+        <v>160</v>
+      </c>
+    </row>
+    <row r="28" spans="1:35" x14ac:dyDescent="0.2">
+      <c r="A28" s="14" t="s">
+        <v>170</v>
+      </c>
+      <c r="B28" s="1" t="s">
+        <v>160</v>
+      </c>
+    </row>
+    <row r="29" spans="1:35" x14ac:dyDescent="0.2">
+      <c r="A29" s="14" t="s">
+        <v>171</v>
+      </c>
+      <c r="B29" s="1" t="s">
+        <v>160</v>
+      </c>
+    </row>
+    <row r="30" spans="1:35" x14ac:dyDescent="0.2">
+      <c r="A30" s="14" t="s">
+        <v>172</v>
+      </c>
+      <c r="B30" s="1" t="s">
+        <v>160</v>
+      </c>
+    </row>
+    <row r="31" spans="1:35" x14ac:dyDescent="0.2">
+      <c r="A31" s="14" t="s">
+        <v>173</v>
+      </c>
+      <c r="B31" s="1" t="s">
+        <v>160</v>
+      </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>